<commit_message>
[IMP] New powerp RC configuration
</commit_message>
<xml_diff>
--- a/z0bug_odoo/data/account_fiscal_position.xlsx
+++ b/z0bug_odoo/data/account_fiscal_position.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -46,6 +46,12 @@
     <t xml:space="preserve">rc_type_id</t>
   </si>
   <si>
+    <t xml:space="preserve">partner_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">self_journal_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.fiscalpos_it</t>
   </si>
   <si>
@@ -68,6 +74,12 @@
   </si>
   <si>
     <t xml:space="preserve">self</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.sale</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.fiscalpos_rc</t>
@@ -188,20 +200,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -229,60 +242,72 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -290,10 +315,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>1</v>
@@ -301,10 +326,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>